<commit_message>
Retraining the model for Imperial
</commit_message>
<xml_diff>
--- a/Imperial/Results_Production_Imperial_xgb.xlsx
+++ b/Imperial/Results_Production_Imperial_xgb.xlsx
@@ -950,7 +950,7 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>0.152</v>
+        <v>0.138</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -964,7 +964,7 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>0.369</v>
+        <v>0.37</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -992,7 +992,7 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>0.919</v>
+        <v>0.882</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>

</xml_diff>